<commit_message>
Week 8 - bs4 & pandas
</commit_message>
<xml_diff>
--- a/week7/panda_only_team_stats.xlsx
+++ b/week7/panda_only_team_stats.xlsx
@@ -14,52 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="120" uniqueCount="67">
-  <si>
-    <t>Unnamed: 0_level_0</t>
-  </si>
-  <si>
-    <t>Unadjusted</t>
-  </si>
-  <si>
-    <t>Adjusted</t>
-  </si>
-  <si>
-    <t>Unnamed: 3_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 4_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 5_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 6_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 7_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 8_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 9_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 10_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 11_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 12_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 13_level_0</t>
-  </si>
-  <si>
-    <t>Unnamed: 14_level_0</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="52">
   <si>
     <t>Rk</t>
   </si>
@@ -572,14 +527,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:P33"/>
+  <dimension ref="A1:P31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
     <row r="1" spans="1:16">
-      <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -627,518 +581,570 @@
       </c>
     </row>
     <row r="2" spans="1:16">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
+      <c r="A2" s="1">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>15</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" t="s">
+        <v>45</v>
+      </c>
+      <c r="E2" t="s">
+        <v>46</v>
+      </c>
+      <c r="F2">
+        <v>60</v>
+      </c>
+      <c r="G2">
+        <v>22</v>
+      </c>
+      <c r="H2">
+        <v>0.732</v>
+      </c>
+      <c r="I2">
+        <v>8.869999999999999</v>
+      </c>
+      <c r="J2">
+        <v>114.23</v>
+      </c>
+      <c r="K2">
+        <v>105.76</v>
+      </c>
+      <c r="L2">
+        <v>8.470000000000001</v>
+      </c>
+      <c r="M2">
+        <v>8.050000000000001</v>
+      </c>
+      <c r="N2">
+        <v>113.89</v>
+      </c>
+      <c r="O2">
+        <v>106.23</v>
+      </c>
+      <c r="P2">
+        <v>7.66</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16">
+      <c r="A3" s="1">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H2" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I2" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="L2" s="1" t="s">
+      <c r="D3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F3">
+        <v>57</v>
+      </c>
+      <c r="G3">
         <v>25</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>29</v>
+      <c r="H3">
+        <v>0.695</v>
+      </c>
+      <c r="I3">
+        <v>6.46</v>
+      </c>
+      <c r="J3">
+        <v>116.63</v>
+      </c>
+      <c r="K3">
+        <v>110.24</v>
+      </c>
+      <c r="L3">
+        <v>6.39</v>
+      </c>
+      <c r="M3">
+        <v>6.42</v>
+      </c>
+      <c r="N3">
+        <v>116.6</v>
+      </c>
+      <c r="O3">
+        <v>110.24</v>
+      </c>
+      <c r="P3">
+        <v>6.37</v>
       </c>
     </row>
     <row r="4" spans="1:16">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="B4">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F4">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="G4">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="H4">
-        <v>0.732</v>
+        <v>0.7070000000000001</v>
       </c>
       <c r="I4">
-        <v>8.869999999999999</v>
+        <v>6.09</v>
       </c>
       <c r="J4">
-        <v>114.23</v>
+        <v>113.99</v>
       </c>
       <c r="K4">
-        <v>105.76</v>
+        <v>108</v>
       </c>
       <c r="L4">
-        <v>8.470000000000001</v>
+        <v>5.99</v>
       </c>
       <c r="M4">
-        <v>8.050000000000001</v>
+        <v>5.49</v>
       </c>
       <c r="N4">
-        <v>113.89</v>
+        <v>113.78</v>
       </c>
       <c r="O4">
-        <v>106.23</v>
+        <v>108.4</v>
       </c>
       <c r="P4">
-        <v>7.66</v>
+        <v>5.38</v>
       </c>
     </row>
     <row r="5" spans="1:16">
       <c r="A5" s="1">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B5">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
       <c r="D5" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F5">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="G5">
-        <v>25</v>
+        <v>32</v>
       </c>
       <c r="H5">
-        <v>0.695</v>
+        <v>0.61</v>
       </c>
       <c r="I5">
-        <v>6.46</v>
+        <v>5.26</v>
       </c>
       <c r="J5">
-        <v>116.63</v>
+        <v>111.35</v>
       </c>
       <c r="K5">
-        <v>110.24</v>
+        <v>106.11</v>
       </c>
       <c r="L5">
-        <v>6.39</v>
+        <v>5.24</v>
       </c>
       <c r="M5">
-        <v>6.42</v>
+        <v>5.29</v>
       </c>
       <c r="N5">
-        <v>116.6</v>
+        <v>111.23</v>
       </c>
       <c r="O5">
-        <v>110.24</v>
+        <v>105.94</v>
       </c>
       <c r="P5">
-        <v>6.37</v>
+        <v>5.28</v>
       </c>
     </row>
     <row r="6" spans="1:16">
       <c r="A6" s="1">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="B6">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D6" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>50</v>
       </c>
       <c r="F6">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="G6">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="H6">
-        <v>0.7070000000000001</v>
+        <v>0.6459999999999999</v>
       </c>
       <c r="I6">
-        <v>6.09</v>
+        <v>4.77</v>
       </c>
       <c r="J6">
-        <v>113.99</v>
+        <v>116.25</v>
       </c>
       <c r="K6">
-        <v>108</v>
+        <v>111.43</v>
       </c>
       <c r="L6">
-        <v>5.99</v>
+        <v>4.82</v>
       </c>
       <c r="M6">
-        <v>5.49</v>
+        <v>4.97</v>
       </c>
       <c r="N6">
-        <v>113.78</v>
+        <v>116.45</v>
       </c>
       <c r="O6">
-        <v>108.4</v>
+        <v>111.43</v>
       </c>
       <c r="P6">
-        <v>5.38</v>
+        <v>5.03</v>
       </c>
     </row>
     <row r="7" spans="1:16">
       <c r="A7" s="1">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="B7">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>20</v>
+      </c>
+      <c r="D7" t="s">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>19</v>
-      </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F7">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="G7">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="H7">
-        <v>0.61</v>
+        <v>0.6459999999999999</v>
       </c>
       <c r="I7">
-        <v>5.26</v>
+        <v>4.2</v>
       </c>
       <c r="J7">
-        <v>111.35</v>
+        <v>115.45</v>
       </c>
       <c r="K7">
-        <v>106.11</v>
+        <v>111.07</v>
       </c>
       <c r="L7">
-        <v>5.24</v>
+        <v>4.38</v>
       </c>
       <c r="M7">
-        <v>5.29</v>
+        <v>4.44</v>
       </c>
       <c r="N7">
-        <v>111.23</v>
+        <v>115.63</v>
       </c>
       <c r="O7">
-        <v>105.94</v>
+        <v>111.01</v>
       </c>
       <c r="P7">
-        <v>5.28</v>
+        <v>4.62</v>
       </c>
     </row>
     <row r="8" spans="1:16">
       <c r="A8" s="1">
+        <v>6</v>
+      </c>
+      <c r="B8">
+        <v>7</v>
+      </c>
+      <c r="C8" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" t="s">
         <v>4</v>
       </c>
-      <c r="B8">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D8" t="s">
-        <v>19</v>
-      </c>
       <c r="E8" t="s">
-        <v>65</v>
+        <v>49</v>
       </c>
       <c r="F8">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="G8">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="H8">
-        <v>0.6459999999999999</v>
+        <v>0.659</v>
       </c>
       <c r="I8">
-        <v>4.77</v>
+        <v>3.95</v>
       </c>
       <c r="J8">
-        <v>116.25</v>
+        <v>113.76</v>
       </c>
       <c r="K8">
-        <v>111.43</v>
+        <v>109.62</v>
       </c>
       <c r="L8">
-        <v>4.82</v>
+        <v>4.14</v>
       </c>
       <c r="M8">
-        <v>4.97</v>
+        <v>4.2</v>
       </c>
       <c r="N8">
-        <v>116.45</v>
+        <v>113.74</v>
       </c>
       <c r="O8">
-        <v>111.43</v>
+        <v>109.35</v>
       </c>
       <c r="P8">
-        <v>5.03</v>
+        <v>4.39</v>
       </c>
     </row>
     <row r="9" spans="1:16">
       <c r="A9" s="1">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="B9">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="D9" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F9">
-        <v>53</v>
+        <v>49</v>
       </c>
       <c r="G9">
-        <v>29</v>
+        <v>33</v>
       </c>
       <c r="H9">
-        <v>0.6459999999999999</v>
+        <v>0.598</v>
       </c>
       <c r="I9">
-        <v>4.2</v>
+        <v>4.44</v>
       </c>
       <c r="J9">
-        <v>115.45</v>
+        <v>112.78</v>
       </c>
       <c r="K9">
-        <v>111.07</v>
+        <v>108.35</v>
       </c>
       <c r="L9">
-        <v>4.38</v>
+        <v>4.43</v>
       </c>
       <c r="M9">
-        <v>4.44</v>
+        <v>3.9</v>
       </c>
       <c r="N9">
-        <v>115.63</v>
+        <v>112.57</v>
       </c>
       <c r="O9">
-        <v>111.01</v>
+        <v>108.69</v>
       </c>
       <c r="P9">
-        <v>4.62</v>
+        <v>3.88</v>
       </c>
     </row>
     <row r="10" spans="1:16">
       <c r="A10" s="1">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="B10">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="D10" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>49</v>
       </c>
       <c r="F10">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="G10">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="H10">
-        <v>0.659</v>
+        <v>0.598</v>
       </c>
       <c r="I10">
-        <v>3.95</v>
+        <v>3.4</v>
       </c>
       <c r="J10">
-        <v>113.76</v>
+        <v>110.85</v>
       </c>
       <c r="K10">
-        <v>109.62</v>
+        <v>107.53</v>
       </c>
       <c r="L10">
-        <v>4.14</v>
+        <v>3.31</v>
       </c>
       <c r="M10">
-        <v>4.2</v>
+        <v>3.56</v>
       </c>
       <c r="N10">
-        <v>113.74</v>
+        <v>110.71</v>
       </c>
       <c r="O10">
-        <v>109.35</v>
+        <v>107.22</v>
       </c>
       <c r="P10">
-        <v>4.39</v>
+        <v>3.49</v>
       </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="1">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="B11">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>37</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E11" t="s">
-        <v>63</v>
+        <v>46</v>
       </c>
       <c r="F11">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G11">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H11">
-        <v>0.598</v>
+        <v>0.585</v>
       </c>
       <c r="I11">
-        <v>4.44</v>
+        <v>3.33</v>
       </c>
       <c r="J11">
-        <v>112.78</v>
+        <v>110.62</v>
       </c>
       <c r="K11">
-        <v>108.35</v>
+        <v>107.23</v>
       </c>
       <c r="L11">
-        <v>4.43</v>
+        <v>3.39</v>
       </c>
       <c r="M11">
-        <v>3.9</v>
+        <v>2.76</v>
       </c>
       <c r="N11">
-        <v>112.57</v>
+        <v>110.31</v>
       </c>
       <c r="O11">
-        <v>108.69</v>
+        <v>107.5</v>
       </c>
       <c r="P11">
-        <v>3.88</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="1">
-        <v>8</v>
+        <v>10</v>
       </c>
       <c r="B12">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="D12" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>48</v>
       </c>
       <c r="F12">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H12">
-        <v>0.598</v>
+        <v>0.622</v>
       </c>
       <c r="I12">
-        <v>3.4</v>
+        <v>2.7</v>
       </c>
       <c r="J12">
-        <v>110.85</v>
+        <v>113.21</v>
       </c>
       <c r="K12">
-        <v>107.53</v>
+        <v>110.58</v>
       </c>
       <c r="L12">
-        <v>3.31</v>
+        <v>2.64</v>
       </c>
       <c r="M12">
-        <v>3.56</v>
+        <v>2.26</v>
       </c>
       <c r="N12">
-        <v>110.71</v>
+        <v>113.16</v>
       </c>
       <c r="O12">
-        <v>107.22</v>
+        <v>110.97</v>
       </c>
       <c r="P12">
-        <v>3.49</v>
+        <v>2.19</v>
       </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="1">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="B13">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
       <c r="D13" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E13" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F13">
         <v>48</v>
@@ -1150,195 +1156,195 @@
         <v>0.585</v>
       </c>
       <c r="I13">
-        <v>3.33</v>
+        <v>1.68</v>
       </c>
       <c r="J13">
-        <v>110.62</v>
+        <v>113.3</v>
       </c>
       <c r="K13">
-        <v>107.23</v>
+        <v>111.55</v>
       </c>
       <c r="L13">
-        <v>3.39</v>
+        <v>1.75</v>
       </c>
       <c r="M13">
-        <v>2.76</v>
+        <v>1.81</v>
       </c>
       <c r="N13">
-        <v>110.31</v>
+        <v>113.3</v>
       </c>
       <c r="O13">
-        <v>107.5</v>
+        <v>111.42</v>
       </c>
       <c r="P13">
-        <v>2.8</v>
+        <v>1.88</v>
       </c>
     </row>
     <row r="14" spans="1:16">
       <c r="A14" s="1">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="B14">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>40</v>
+        <v>27</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E14" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F14">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="G14">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H14">
-        <v>0.622</v>
+        <v>0.585</v>
       </c>
       <c r="I14">
-        <v>2.7</v>
+        <v>0.85</v>
       </c>
       <c r="J14">
-        <v>113.21</v>
+        <v>113.14</v>
       </c>
       <c r="K14">
-        <v>110.58</v>
+        <v>112.33</v>
       </c>
       <c r="L14">
-        <v>2.64</v>
+        <v>0.8100000000000001</v>
       </c>
       <c r="M14">
-        <v>2.26</v>
+        <v>1.09</v>
       </c>
       <c r="N14">
-        <v>113.16</v>
+        <v>113.29</v>
       </c>
       <c r="O14">
-        <v>110.97</v>
+        <v>112.22</v>
       </c>
       <c r="P14">
-        <v>2.19</v>
+        <v>1.06</v>
       </c>
     </row>
     <row r="15" spans="1:16">
       <c r="A15" s="1">
-        <v>11</v>
+        <v>13</v>
       </c>
       <c r="B15">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D15" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F15">
-        <v>48</v>
+        <v>42</v>
       </c>
       <c r="G15">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="H15">
-        <v>0.585</v>
+        <v>0.512</v>
       </c>
       <c r="I15">
-        <v>1.68</v>
+        <v>0.71</v>
       </c>
       <c r="J15">
-        <v>113.3</v>
+        <v>109.46</v>
       </c>
       <c r="K15">
-        <v>111.55</v>
+        <v>108.82</v>
       </c>
       <c r="L15">
-        <v>1.75</v>
+        <v>0.65</v>
       </c>
       <c r="M15">
-        <v>1.81</v>
+        <v>0.28</v>
       </c>
       <c r="N15">
-        <v>113.3</v>
+        <v>109.26</v>
       </c>
       <c r="O15">
-        <v>111.42</v>
+        <v>109.05</v>
       </c>
       <c r="P15">
-        <v>1.88</v>
+        <v>0.21</v>
       </c>
     </row>
     <row r="16" spans="1:16">
       <c r="A16" s="1">
-        <v>12</v>
+        <v>14</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="C16" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="D16" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>62</v>
+        <v>51</v>
       </c>
       <c r="F16">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="G16">
-        <v>34</v>
+        <v>43</v>
       </c>
       <c r="H16">
-        <v>0.585</v>
+        <v>0.476</v>
       </c>
       <c r="I16">
-        <v>0.85</v>
+        <v>-0.23</v>
       </c>
       <c r="J16">
-        <v>113.14</v>
+        <v>108.22</v>
       </c>
       <c r="K16">
-        <v>112.33</v>
+        <v>108.35</v>
       </c>
       <c r="L16">
-        <v>0.8100000000000001</v>
+        <v>-0.13</v>
       </c>
       <c r="M16">
-        <v>1.09</v>
+        <v>-0.45</v>
       </c>
       <c r="N16">
-        <v>113.29</v>
+        <v>108.03</v>
       </c>
       <c r="O16">
-        <v>112.22</v>
+        <v>108.39</v>
       </c>
       <c r="P16">
-        <v>1.06</v>
+        <v>-0.36</v>
       </c>
     </row>
     <row r="17" spans="1:16">
       <c r="A17" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B17">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="C17" t="s">
-        <v>43</v>
+        <v>30</v>
       </c>
       <c r="D17" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>66</v>
+        <v>48</v>
       </c>
       <c r="F17">
         <v>42</v>
@@ -1350,245 +1356,245 @@
         <v>0.512</v>
       </c>
       <c r="I17">
-        <v>0.71</v>
+        <v>-0.07000000000000001</v>
       </c>
       <c r="J17">
-        <v>109.46</v>
+        <v>110.3</v>
       </c>
       <c r="K17">
-        <v>108.82</v>
+        <v>110.36</v>
       </c>
       <c r="L17">
-        <v>0.65</v>
+        <v>-0.06</v>
       </c>
       <c r="M17">
-        <v>0.28</v>
+        <v>-0.4</v>
       </c>
       <c r="N17">
-        <v>109.26</v>
+        <v>110.15</v>
       </c>
       <c r="O17">
-        <v>109.05</v>
+        <v>110.56</v>
       </c>
       <c r="P17">
-        <v>0.21</v>
+        <v>-0.41</v>
       </c>
     </row>
     <row r="18" spans="1:16">
       <c r="A18" s="1">
-        <v>14</v>
+        <v>16</v>
       </c>
       <c r="B18">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="C18" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="D18" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E18" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="F18">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G18">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H18">
-        <v>0.476</v>
+        <v>0.5</v>
       </c>
       <c r="I18">
-        <v>-0.23</v>
+        <v>-0.24</v>
       </c>
       <c r="J18">
-        <v>108.22</v>
+        <v>109.93</v>
       </c>
       <c r="K18">
-        <v>108.35</v>
+        <v>110.13</v>
       </c>
       <c r="L18">
-        <v>-0.13</v>
+        <v>-0.2</v>
       </c>
       <c r="M18">
-        <v>-0.45</v>
+        <v>-0.55</v>
       </c>
       <c r="N18">
-        <v>108.03</v>
+        <v>109.86</v>
       </c>
       <c r="O18">
-        <v>108.39</v>
+        <v>110.38</v>
       </c>
       <c r="P18">
-        <v>-0.36</v>
+        <v>-0.53</v>
       </c>
     </row>
     <row r="19" spans="1:16">
       <c r="A19" s="1">
-        <v>15</v>
+        <v>17</v>
       </c>
       <c r="B19">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="C19" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="D19" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E19" t="s">
-        <v>63</v>
+        <v>47</v>
       </c>
       <c r="F19">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="G19">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="H19">
-        <v>0.512</v>
+        <v>0.476</v>
       </c>
       <c r="I19">
-        <v>-0.07000000000000001</v>
+        <v>-1.12</v>
       </c>
       <c r="J19">
-        <v>110.3</v>
+        <v>111.17</v>
       </c>
       <c r="K19">
-        <v>110.36</v>
+        <v>112.19</v>
       </c>
       <c r="L19">
-        <v>-0.06</v>
+        <v>-1.02</v>
       </c>
       <c r="M19">
-        <v>-0.4</v>
+        <v>-0.8100000000000001</v>
       </c>
       <c r="N19">
-        <v>110.15</v>
+        <v>111.29</v>
       </c>
       <c r="O19">
-        <v>110.56</v>
+        <v>112</v>
       </c>
       <c r="P19">
-        <v>-0.41</v>
+        <v>-0.71</v>
       </c>
     </row>
     <row r="20" spans="1:16">
       <c r="A20" s="1">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="B20">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
       <c r="D20" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E20" t="s">
-        <v>61</v>
+        <v>50</v>
       </c>
       <c r="F20">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="G20">
-        <v>41</v>
+        <v>49</v>
       </c>
       <c r="H20">
-        <v>0.5</v>
+        <v>0.402</v>
       </c>
       <c r="I20">
-        <v>-0.24</v>
+        <v>-1.28</v>
       </c>
       <c r="J20">
-        <v>109.93</v>
+        <v>110.19</v>
       </c>
       <c r="K20">
-        <v>110.13</v>
+        <v>111.41</v>
       </c>
       <c r="L20">
-        <v>-0.2</v>
+        <v>-1.22</v>
       </c>
       <c r="M20">
-        <v>-0.55</v>
+        <v>-0.86</v>
       </c>
       <c r="N20">
-        <v>109.86</v>
+        <v>110.29</v>
       </c>
       <c r="O20">
-        <v>110.38</v>
+        <v>111.08</v>
       </c>
       <c r="P20">
-        <v>-0.53</v>
+        <v>-0.79</v>
       </c>
     </row>
     <row r="21" spans="1:16">
       <c r="A21" s="1">
-        <v>17</v>
+        <v>19</v>
       </c>
       <c r="B21">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="C21" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="D21" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E21" t="s">
-        <v>62</v>
+        <v>49</v>
       </c>
       <c r="F21">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="G21">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="H21">
-        <v>0.476</v>
+        <v>0.439</v>
       </c>
       <c r="I21">
-        <v>-1.12</v>
+        <v>-1.5</v>
       </c>
       <c r="J21">
-        <v>111.17</v>
+        <v>112.04</v>
       </c>
       <c r="K21">
-        <v>112.19</v>
+        <v>113.54</v>
       </c>
       <c r="L21">
+        <v>-1.51</v>
+      </c>
+      <c r="M21">
         <v>-1.02</v>
       </c>
-      <c r="M21">
-        <v>-0.8100000000000001</v>
-      </c>
       <c r="N21">
-        <v>111.29</v>
+        <v>112.31</v>
       </c>
       <c r="O21">
-        <v>112</v>
+        <v>113.32</v>
       </c>
       <c r="P21">
-        <v>-0.71</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="22" spans="1:16">
       <c r="A22" s="1">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B22">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="C22" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="D22" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E22" t="s">
-        <v>65</v>
+        <v>50</v>
       </c>
       <c r="F22">
         <v>33</v>
@@ -1600,445 +1606,445 @@
         <v>0.402</v>
       </c>
       <c r="I22">
-        <v>-1.28</v>
+        <v>-1.33</v>
       </c>
       <c r="J22">
-        <v>110.19</v>
+        <v>111.85</v>
       </c>
       <c r="K22">
-        <v>111.41</v>
+        <v>113.1</v>
       </c>
       <c r="L22">
-        <v>-1.22</v>
+        <v>-1.25</v>
       </c>
       <c r="M22">
-        <v>-0.86</v>
+        <v>-1.1</v>
       </c>
       <c r="N22">
-        <v>110.29</v>
+        <v>111.98</v>
       </c>
       <c r="O22">
-        <v>111.08</v>
+        <v>112.98</v>
       </c>
       <c r="P22">
-        <v>-0.79</v>
+        <v>-1.01</v>
       </c>
     </row>
     <row r="23" spans="1:16">
       <c r="A23" s="1">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="B23">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C23" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D23" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E23" t="s">
-        <v>64</v>
+        <v>47</v>
       </c>
       <c r="F23">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="G23">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="H23">
-        <v>0.439</v>
+        <v>0.451</v>
       </c>
       <c r="I23">
-        <v>-1.5</v>
+        <v>-1.72</v>
       </c>
       <c r="J23">
-        <v>112.04</v>
+        <v>108.52</v>
       </c>
       <c r="K23">
-        <v>113.54</v>
+        <v>110.18</v>
       </c>
       <c r="L23">
-        <v>-1.51</v>
+        <v>-1.66</v>
       </c>
       <c r="M23">
-        <v>-1.02</v>
+        <v>-1.32</v>
       </c>
       <c r="N23">
-        <v>112.31</v>
+        <v>108.46</v>
       </c>
       <c r="O23">
-        <v>113.32</v>
+        <v>109.71</v>
       </c>
       <c r="P23">
-        <v>-1.01</v>
+        <v>-1.26</v>
       </c>
     </row>
     <row r="24" spans="1:16">
       <c r="A24" s="1">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="B24">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="C24" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D24" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E24" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="F24">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="G24">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="H24">
-        <v>0.402</v>
+        <v>0.476</v>
       </c>
       <c r="I24">
-        <v>-1.33</v>
+        <v>-1.1</v>
       </c>
       <c r="J24">
-        <v>111.85</v>
+        <v>112.1</v>
       </c>
       <c r="K24">
-        <v>113.1</v>
+        <v>113.16</v>
       </c>
       <c r="L24">
-        <v>-1.25</v>
+        <v>-1.06</v>
       </c>
       <c r="M24">
-        <v>-1.1</v>
+        <v>-1.31</v>
       </c>
       <c r="N24">
-        <v>111.98</v>
+        <v>112.11</v>
       </c>
       <c r="O24">
-        <v>112.98</v>
+        <v>113.41</v>
       </c>
       <c r="P24">
-        <v>-1.01</v>
+        <v>-1.3</v>
       </c>
     </row>
     <row r="25" spans="1:16">
       <c r="A25" s="1">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B25">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="D25" t="s">
-        <v>19</v>
+        <v>4</v>
       </c>
       <c r="E25" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="F25">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G25">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="H25">
-        <v>0.451</v>
+        <v>0.402</v>
       </c>
       <c r="I25">
-        <v>-1.72</v>
+        <v>-2.6</v>
       </c>
       <c r="J25">
-        <v>108.52</v>
+        <v>106.96</v>
       </c>
       <c r="K25">
-        <v>110.18</v>
+        <v>109.66</v>
       </c>
       <c r="L25">
-        <v>-1.66</v>
+        <v>-2.7</v>
       </c>
       <c r="M25">
-        <v>-1.32</v>
+        <v>-2.08</v>
       </c>
       <c r="N25">
-        <v>108.46</v>
+        <v>106.93</v>
       </c>
       <c r="O25">
-        <v>109.71</v>
+        <v>109.09</v>
       </c>
       <c r="P25">
-        <v>-1.26</v>
+        <v>-2.17</v>
       </c>
     </row>
     <row r="26" spans="1:16">
       <c r="A26" s="1">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C26" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="D26" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E26" t="s">
-        <v>66</v>
+        <v>51</v>
       </c>
       <c r="F26">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="G26">
-        <v>43</v>
+        <v>50</v>
       </c>
       <c r="H26">
-        <v>0.476</v>
+        <v>0.39</v>
       </c>
       <c r="I26">
-        <v>-1.1</v>
+        <v>-2.9</v>
       </c>
       <c r="J26">
-        <v>112.1</v>
+        <v>111.72</v>
       </c>
       <c r="K26">
-        <v>113.16</v>
+        <v>114.56</v>
       </c>
       <c r="L26">
-        <v>-1.06</v>
+        <v>-2.84</v>
       </c>
       <c r="M26">
-        <v>-1.31</v>
+        <v>-3.3</v>
       </c>
       <c r="N26">
-        <v>112.11</v>
+        <v>111.72</v>
       </c>
       <c r="O26">
-        <v>113.41</v>
+        <v>114.97</v>
       </c>
       <c r="P26">
-        <v>-1.3</v>
+        <v>-3.25</v>
       </c>
     </row>
     <row r="27" spans="1:16">
       <c r="A27" s="1">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="B27">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C27" t="s">
+        <v>40</v>
+      </c>
+      <c r="D27" t="s">
+        <v>45</v>
+      </c>
+      <c r="E27" t="s">
+        <v>51</v>
+      </c>
+      <c r="F27">
+        <v>29</v>
+      </c>
+      <c r="G27">
         <v>53</v>
       </c>
-      <c r="D27" t="s">
-        <v>19</v>
-      </c>
-      <c r="E27" t="s">
-        <v>65</v>
-      </c>
-      <c r="F27">
-        <v>33</v>
-      </c>
-      <c r="G27">
-        <v>49</v>
-      </c>
       <c r="H27">
-        <v>0.402</v>
+        <v>0.354</v>
       </c>
       <c r="I27">
-        <v>-2.6</v>
+        <v>-6.02</v>
       </c>
       <c r="J27">
-        <v>106.96</v>
+        <v>108.71</v>
       </c>
       <c r="K27">
-        <v>109.66</v>
+        <v>114.41</v>
       </c>
       <c r="L27">
-        <v>-2.7</v>
+        <v>-5.7</v>
       </c>
       <c r="M27">
-        <v>-2.08</v>
+        <v>-6.06</v>
       </c>
       <c r="N27">
-        <v>106.93</v>
+        <v>108.83</v>
       </c>
       <c r="O27">
-        <v>109.09</v>
+        <v>114.59</v>
       </c>
       <c r="P27">
-        <v>-2.17</v>
+        <v>-5.76</v>
       </c>
     </row>
     <row r="28" spans="1:16">
       <c r="A28" s="1">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B28">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C28" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="D28" t="s">
+        <v>45</v>
+      </c>
+      <c r="E28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28">
+        <v>22</v>
+      </c>
+      <c r="G28">
         <v>60</v>
       </c>
-      <c r="E28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F28">
-        <v>32</v>
-      </c>
-      <c r="G28">
-        <v>50</v>
-      </c>
       <c r="H28">
-        <v>0.39</v>
+        <v>0.268</v>
       </c>
       <c r="I28">
-        <v>-2.9</v>
+        <v>-8.41</v>
       </c>
       <c r="J28">
-        <v>111.72</v>
+        <v>105.45</v>
       </c>
       <c r="K28">
-        <v>114.56</v>
+        <v>113.94</v>
       </c>
       <c r="L28">
-        <v>-2.84</v>
+        <v>-8.49</v>
       </c>
       <c r="M28">
-        <v>-3.3</v>
+        <v>-8.32</v>
       </c>
       <c r="N28">
-        <v>111.72</v>
+        <v>105.49</v>
       </c>
       <c r="O28">
-        <v>114.97</v>
+        <v>113.9</v>
       </c>
       <c r="P28">
-        <v>-3.25</v>
+        <v>-8.41</v>
       </c>
     </row>
     <row r="29" spans="1:16">
       <c r="A29" s="1">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="B29">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="C29" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="D29" t="s">
-        <v>60</v>
+        <v>4</v>
       </c>
       <c r="E29" t="s">
-        <v>66</v>
+        <v>47</v>
       </c>
       <c r="F29">
-        <v>29</v>
+        <v>19</v>
       </c>
       <c r="G29">
-        <v>53</v>
+        <v>63</v>
       </c>
       <c r="H29">
-        <v>0.354</v>
+        <v>0.232</v>
       </c>
       <c r="I29">
-        <v>-6.02</v>
+        <v>-9.34</v>
       </c>
       <c r="J29">
-        <v>108.71</v>
+        <v>106.29</v>
       </c>
       <c r="K29">
-        <v>114.41</v>
+        <v>115.55</v>
       </c>
       <c r="L29">
-        <v>-5.7</v>
+        <v>-9.26</v>
       </c>
       <c r="M29">
-        <v>-6.06</v>
+        <v>-8.609999999999999</v>
       </c>
       <c r="N29">
-        <v>108.83</v>
+        <v>106.59</v>
       </c>
       <c r="O29">
-        <v>114.59</v>
+        <v>115.11</v>
       </c>
       <c r="P29">
-        <v>-5.76</v>
+        <v>-8.52</v>
       </c>
     </row>
     <row r="30" spans="1:16">
       <c r="A30" s="1">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B30">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="C30" t="s">
-        <v>56</v>
+        <v>43</v>
       </c>
       <c r="D30" t="s">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="E30" t="s">
-        <v>61</v>
+        <v>48</v>
       </c>
       <c r="F30">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="G30">
-        <v>60</v>
+        <v>65</v>
       </c>
       <c r="H30">
-        <v>0.268</v>
+        <v>0.207</v>
       </c>
       <c r="I30">
-        <v>-8.41</v>
+        <v>-9.210000000000001</v>
       </c>
       <c r="J30">
-        <v>105.45</v>
+        <v>105.13</v>
       </c>
       <c r="K30">
-        <v>113.94</v>
+        <v>114.39</v>
       </c>
       <c r="L30">
-        <v>-8.49</v>
+        <v>-9.26</v>
       </c>
       <c r="M30">
-        <v>-8.32</v>
+        <v>-8.92</v>
       </c>
       <c r="N30">
-        <v>105.49</v>
+        <v>105.31</v>
       </c>
       <c r="O30">
-        <v>113.9</v>
+        <v>114.3</v>
       </c>
       <c r="P30">
-        <v>-8.41</v>
+        <v>-8.98</v>
       </c>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="1">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B31">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="C31" t="s">
-        <v>57</v>
+        <v>44</v>
       </c>
       <c r="D31" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
       <c r="E31" t="s">
-        <v>62</v>
+        <v>46</v>
       </c>
       <c r="F31">
         <v>19</v>
@@ -2050,127 +2056,27 @@
         <v>0.232</v>
       </c>
       <c r="I31">
-        <v>-9.34</v>
+        <v>-9.609999999999999</v>
       </c>
       <c r="J31">
-        <v>106.29</v>
+        <v>108.5</v>
       </c>
       <c r="K31">
-        <v>115.55</v>
+        <v>118.54</v>
       </c>
       <c r="L31">
-        <v>-9.26</v>
+        <v>-10.04</v>
       </c>
       <c r="M31">
-        <v>-8.609999999999999</v>
+        <v>-9.390000000000001</v>
       </c>
       <c r="N31">
-        <v>106.59</v>
+        <v>108.83</v>
       </c>
       <c r="O31">
-        <v>115.11</v>
+        <v>118.64</v>
       </c>
       <c r="P31">
-        <v>-8.52</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16">
-      <c r="A32" s="1">
-        <v>28</v>
-      </c>
-      <c r="B32">
-        <v>29</v>
-      </c>
-      <c r="C32" t="s">
-        <v>58</v>
-      </c>
-      <c r="D32" t="s">
-        <v>60</v>
-      </c>
-      <c r="E32" t="s">
-        <v>63</v>
-      </c>
-      <c r="F32">
-        <v>17</v>
-      </c>
-      <c r="G32">
-        <v>65</v>
-      </c>
-      <c r="H32">
-        <v>0.207</v>
-      </c>
-      <c r="I32">
-        <v>-9.210000000000001</v>
-      </c>
-      <c r="J32">
-        <v>105.13</v>
-      </c>
-      <c r="K32">
-        <v>114.39</v>
-      </c>
-      <c r="L32">
-        <v>-9.26</v>
-      </c>
-      <c r="M32">
-        <v>-8.92</v>
-      </c>
-      <c r="N32">
-        <v>105.31</v>
-      </c>
-      <c r="O32">
-        <v>114.3</v>
-      </c>
-      <c r="P32">
-        <v>-8.98</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16">
-      <c r="A33" s="1">
-        <v>29</v>
-      </c>
-      <c r="B33">
-        <v>30</v>
-      </c>
-      <c r="C33" t="s">
-        <v>59</v>
-      </c>
-      <c r="D33" t="s">
-        <v>60</v>
-      </c>
-      <c r="E33" t="s">
-        <v>61</v>
-      </c>
-      <c r="F33">
-        <v>19</v>
-      </c>
-      <c r="G33">
-        <v>63</v>
-      </c>
-      <c r="H33">
-        <v>0.232</v>
-      </c>
-      <c r="I33">
-        <v>-9.609999999999999</v>
-      </c>
-      <c r="J33">
-        <v>108.5</v>
-      </c>
-      <c r="K33">
-        <v>118.54</v>
-      </c>
-      <c r="L33">
-        <v>-10.04</v>
-      </c>
-      <c r="M33">
-        <v>-9.390000000000001</v>
-      </c>
-      <c r="N33">
-        <v>108.83</v>
-      </c>
-      <c r="O33">
-        <v>118.64</v>
-      </c>
-      <c r="P33">
         <v>-9.82</v>
       </c>
     </row>

</xml_diff>